<commit_message>
changed file structure, working on increasing power of column name finder column display currently disabled
</commit_message>
<xml_diff>
--- a/demo book.xlsx
+++ b/demo book.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\OneDrive\Documents\Angular\One Connect Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/940fbed32182cd0a/Documents/Angular/One Connect Solutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>no</t>
   </si>
   <si>
     <t>non</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Dates</t>
   </si>
 </sst>
 </file>
@@ -65,9 +78,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,40 +364,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>42005</v>
-      </c>
-      <c r="B1" s="1">
-        <v>42006</v>
-      </c>
-      <c r="C1" s="1">
-        <v>42007</v>
-      </c>
-      <c r="D1" s="1">
-        <v>42008</v>
-      </c>
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
+      <c r="A2" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42006</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42007</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42008</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -392,10 +402,53 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>